<commit_message>
Added shorter explanations in the base worksheet
</commit_message>
<xml_diff>
--- a/Key climate votes v2.xlsx
+++ b/Key climate votes v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurence\Google Drive\EU Hackday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurence\Google Drive\EU Hackday\scoringep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc374534722" localSheetId="0">Sheet1!$A$4</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="150">
   <si>
     <t>Title</t>
   </si>
@@ -428,12 +429,253 @@
   <si>
     <t>Laurence's Weighting</t>
   </si>
+  <si>
+    <t>B7-0482/2013 - Amendment 5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6. Welcomes the proposal by Ban-Ki Moon to hold a world leaders’ climate summit in September 2014, as well as a people’s pre-COP in 2014 in Venezuela; emphasises the importance of a well-prepared event with meaningful outcomes and engagement at the highest political level and with civil society, in order to secure and maintain the necessary political momentum ahead of the 2014 and 2015 Conferences; deems it necessary for a successful 2015 agreement that countries come forward with greenhouse gas reduction commitments before the world leaders’ summit; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>stresses that the EU must set an example and adopt ambitious 2030 targets for greenhouse gas reductions, energy efficiency and renewable energy in time for the summit;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Welcomes the proposal by Ban-Ki Moon to hold a world leaders’ climate summit in September 2014, as well as a people’s pre-COP in 2014 in Venezuela; emphasises the importance of a well-prepared event with meaningful outcomes and engagement at the highest political level and with civil society, in order to secure and maintain the necessary political momentum ahead of the 2014 and 2015 Conferences; deems it necessary for a successful 2015 agreement that countries come forward with greenhouse gas reduction commitments before the world leaders’ summit; </t>
+  </si>
+  <si>
+    <t>Ambitious 2030 targets for the EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Recognises the benefits that Member States derive from working together for an energy system transformation; endorses, therefore, the Commission’s Energy Roadmap 2050 as a basis for proposing legislative and other initiatives on energy policy with a view to developing a policy framework for 2030, including milestones and targets on greenhouse gas emissions, renewable energy and energy efficiency, with the aim of establishing an ambitious and stable legal and regulatory framework; notes that defining energy targets for 2050 and the intervening period assumes pan-European governance; proposes the adoption, within the spirit of solidarity, of a strategy that allows Member States to cooperate under the Roadmap in a spirit of solidarity – the creation of a European Energy Community; encourages work to define the 2030 policy framework within a timeframe that is appropriate for providing investor security; </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Recognises the benefits that Member States derive from working together for an energy system transformation; endorses, therefore, the Commission’s Energy Roadmap 2050 as a basis for proposing legislative and other initiatives on energy policy with a view to developing a policy framework for 2030, including milestones and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">binding </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>targets on greenhouse gas emissions, renewable energy and energy efficiency, with the aim of establishing an ambitious and stable legal and regulatory framework; notes that defining energy targets for 2050 and the intervening period assumes pan-European governance; proposes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>the adoption, within the spirit of solidarity, of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a strategy that allows Member States to cooperate under the Roadmap</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in a spirit of solidarity – the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>creation of a European Energy Community; encourages work to define the 2030 policy framework within a timeframe that is appropriate for providing investor security;</t>
+    </r>
+  </si>
+  <si>
+    <t>DB ID</t>
+  </si>
+  <si>
+    <t>An Ambitious EU 2030 Package</t>
+  </si>
+  <si>
+    <t>http://www.votewatch.eu/en/climate-change-conference-motion-for-resolution-paragraph-6-amendment-5.html</t>
+  </si>
+  <si>
+    <t>3 Binding Targets on the Roadmap to 2050</t>
+  </si>
+  <si>
+    <t>2012/2103(INI)</t>
+  </si>
+  <si>
+    <t>A7-0035/2013 - Niki Tzavela - Amendment 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binding EU Renewable Energy Targets of 45% </t>
+  </si>
+  <si>
+    <t>3 Binding Targets on the 2050 Roadmap</t>
+  </si>
+  <si>
+    <t>A7-0135/2013 - Herbert Reul - Am 1/2</t>
+  </si>
+  <si>
+    <t>Voting Recommendation</t>
+  </si>
+  <si>
+    <t>Renewable energy in the European internal energy market</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Laurence's Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To keep the world from warming more than 2C, climate science and effort-sharing models recommend the EU should have greenhouse gas reduction targets of at least -55% by 2030. </t>
+  </si>
+  <si>
+    <t>The EU's 2020 climate targets allows emissions to grow! http://www.sandbag.org.uk/blog/2013/dec/9/eus-2020-targets-allow-massive-growth-emissions-em/ The targets need to be accordingly more ambitious to take into account current progress.</t>
+  </si>
+  <si>
+    <t>A global agreement at Copenhagen in 2009 would have been a big step in the right direction. Unfortunately, the negotiations ultimately fell through. The EU position ahead of the conference was important groundwork.</t>
+  </si>
+  <si>
+    <t>In order to reduce greenhoues gas emissions across Europe, there must be standards for monitoring and reporting them.</t>
+  </si>
+  <si>
+    <t>The EU carbon market has been sorely in need of reform for many years now - an agreement to temporarily withhold allowances was a small step in the right direction.</t>
+  </si>
+  <si>
+    <t>Climate change will disproportionately impact the world's poorest, so it is essential that climate change considerations are integrated in development policy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed countries have promised to provide $100bn /yr by 2020 to support developing countries fighting climate change impacts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reducing energy consumption is a very effective and cheap way to reduce greenhouse gas emissions along with other benefits. </t>
+  </si>
+  <si>
+    <t>An EU greenhouse gas reduction target of 50% by 2030</t>
+  </si>
+  <si>
+    <t>A legally binding, global agreement on climate change</t>
+  </si>
+  <si>
+    <t>Increasing 2020 emissions reductions targets to 30%</t>
+  </si>
+  <si>
+    <t>Reporting greenhouse gas emissions across Europe</t>
+  </si>
+  <si>
+    <t>Back-loading' the Emissions Trading System</t>
+  </si>
+  <si>
+    <t>Climate change in Development policies</t>
+  </si>
+  <si>
+    <t>Climate finance for the world's poorest</t>
+  </si>
+  <si>
+    <t>Measures to reduce energy consumption</t>
+  </si>
+  <si>
+    <t>Increasing European renewable energy</t>
+  </si>
+  <si>
+    <t>Increasing the share of renewables is crucial in the transition to a low-carbon future. Ambitious targets are needed to secure this as a policy.</t>
+  </si>
+  <si>
+    <t>Stop subsidising polluting fossil fuels</t>
+  </si>
+  <si>
+    <t>Subsidies still support fossil fuels. Money used to support these polluting fuels could be used to support climate  action.</t>
+  </si>
+  <si>
+    <t>A7-0035/2013 - Niki Tzavela - Am 1</t>
+  </si>
+  <si>
+    <t>A global agreement at Copenhagen in 2009 would have been a big step in the right direction. These hopes ultimately floundered. The EU position ahead of the conference was important groundwork.</t>
+  </si>
+  <si>
+    <t>In order to reduce greenhoues gas emissions across Europe, there must be firm standards for carbon accounting.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +739,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2E74B5"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -519,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -561,6 +823,28 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,34 +1127,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="99.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="99.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.21875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="66.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84.88671875" customWidth="1"/>
-    <col min="12" max="12" width="57.44140625" customWidth="1"/>
-    <col min="13" max="13" width="38.33203125" customWidth="1"/>
-    <col min="14" max="14" width="74.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="113.6640625" customWidth="1"/>
-    <col min="16" max="16" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="62.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="69.77734375" customWidth="1"/>
+    <col min="8" max="8" width="51" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="66.21875" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="14" max="14" width="51.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="84.88671875" customWidth="1"/>
+    <col min="16" max="16" width="57.44140625" customWidth="1"/>
+    <col min="17" max="17" width="38.33203125" customWidth="1"/>
+    <col min="18" max="18" width="74.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="113.6640625" customWidth="1"/>
+    <col min="20" max="20" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="62.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -880,50 +1166,59 @@
       <c r="C1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -933,50 +1228,60 @@
       <c r="C2" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2">
+      <c r="L2" s="2">
         <v>41570</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -986,50 +1291,59 @@
       <c r="C3" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="14">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
         <v>0.8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="2">
+      <c r="L3" s="2">
         <v>40983</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>37</v>
       </c>
@@ -1039,44 +1353,53 @@
       <c r="C4" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="14">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14">
         <v>0.9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="2">
+      <c r="L4" s="2">
         <v>40142</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>21</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>43</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>44</v>
       </c>
@@ -1086,44 +1409,53 @@
       <c r="C5" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="14">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="2">
+      <c r="L5" s="2">
         <v>41345</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>21</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1133,44 +1465,53 @@
       <c r="C6" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="14">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14">
         <v>0.8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" t="s">
         <v>46</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="2">
+      <c r="L6" s="2">
         <v>41458</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>21</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
@@ -1180,44 +1521,53 @@
       <c r="C7" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="14">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14">
         <v>0.6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="2">
+      <c r="L7" s="2">
         <v>40815</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N7" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>21</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="T7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>60</v>
       </c>
@@ -1227,47 +1577,56 @@
       <c r="C8" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="14">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14">
         <v>0.4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="2">
+      <c r="L8" s="2">
         <v>40863</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8" t="s">
         <v>63</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O8" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q8" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="U8" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>67</v>
       </c>
@@ -1277,47 +1636,56 @@
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="14">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
         <v>0.4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I9" t="s">
         <v>46</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="2">
+      <c r="L9" s="2">
         <v>41163</v>
       </c>
-      <c r="I9" t="s">
+      <c r="M9" t="s">
         <v>48</v>
       </c>
-      <c r="J9" t="s">
+      <c r="N9" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
         <v>21</v>
       </c>
-      <c r="N9" t="s">
+      <c r="R9" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="T9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -1327,50 +1695,59 @@
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="14">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
         <v>0.5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="K10" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="2">
+      <c r="L10" s="2">
         <v>41415</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="N10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K10" t="s">
+      <c r="O10" t="s">
         <v>76</v>
       </c>
-      <c r="L10" t="s">
+      <c r="P10" t="s">
         <v>77</v>
       </c>
-      <c r="M10" t="s">
+      <c r="Q10" t="s">
         <v>21</v>
       </c>
-      <c r="N10" t="s">
+      <c r="R10" t="s">
         <v>78</v>
       </c>
-      <c r="O10" t="s">
+      <c r="S10" t="s">
         <v>79</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="T10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>80</v>
       </c>
@@ -1380,77 +1757,319 @@
       <c r="C11" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="14">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
         <v>0.5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="2">
+      <c r="L11" s="2">
         <v>41570</v>
       </c>
-      <c r="I11" t="s">
+      <c r="M11" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K11" t="s">
+      <c r="O11" t="s">
         <v>84</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>21</v>
       </c>
-      <c r="N11" t="s">
+      <c r="R11" t="s">
         <v>85</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="U11" s="3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12">
+        <v>4994</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="K12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" s="2">
+        <v>41570</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13">
+        <v>3939</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="J13" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="2">
+        <v>41346</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14">
+        <v>4097</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" t="s">
+        <v>124</v>
+      </c>
+      <c r="L14" s="2">
+        <v>41415</v>
+      </c>
+      <c r="R14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+AMD+B7-2013-0482+004-010+DOC+PDF+V0//EN"/>
-    <hyperlink ref="P2" r:id="rId2" display="http://www.votewatch.eu/en/climate-change-conference-motion-for-resolution-paragraph-8-amendment-6d.html"/>
-    <hyperlink ref="Q2" r:id="rId3" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20131023+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="K4" r:id="rId4" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2009-0089&amp;language=EN&amp;ring=B7-2009-0141"/>
-    <hyperlink ref="K5" r:id="rId5" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2013-0064&amp;language=EN&amp;ring=A7-2012-0191"/>
-    <hyperlink ref="P5" r:id="rId6" display="http://www.votewatch.eu/en/mechanism-for-monitoring-and-reporting-greenhouse-gas-emissions-and-other-information-relevant-to-cl.html"/>
-    <hyperlink ref="Q5" r:id="rId7" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130312+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="P4" r:id="rId8" display="http://www.votewatch.eu/en/motion-for-a-resolution-preparation-of-the-copenhagen-summit-on-climate-change-motions-for-a-resolut-19.html"/>
-    <hyperlink ref="Q4" r:id="rId9" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20091125+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="P3" r:id="rId10" display="http://www.votewatch.eu/en/competitive-low-carbon-economy-in-2050-motion-for-a-resolution-after-paragraph-1-amendment-1-2.html"/>
-    <hyperlink ref="Q3" r:id="rId11" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20120315+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="J6" r:id="rId12" display="http://www.europarl.europa.eu/sides/getDoc.do?type=REPORT&amp;reference=A7-2013-0046&amp;language=EN"/>
-    <hyperlink ref="K6" r:id="rId13" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2013-0310&amp;language=EN&amp;ring=A7-2013-0046"/>
-    <hyperlink ref="P6" r:id="rId14" display="http://www.votewatch.eu/en/timing-of-auctions-of-greenhouse-gas-allowances-draft-legislative-resolution-vote-amended-proposal-o.html"/>
-    <hyperlink ref="Q6" r:id="rId15" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130703+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="K7" r:id="rId16" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2011-0430&amp;language=EN&amp;ring=B7-2011-0522"/>
-    <hyperlink ref="P7" r:id="rId17" display="http://www.votewatch.eu/en/motions-for-resolutions-rio-20-earth-summit-motion-for-a-resolution-vote-resolution-text-as-a-whole.html"/>
-    <hyperlink ref="Q7" r:id="rId18" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20110929+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="G8" r:id="rId19" display="http://www.europarl.europa.eu/sides/getDoc.do?type=MOTION&amp;reference=B7-2011-0571&amp;language=EN"/>
-    <hyperlink ref="P8" r:id="rId20" display="http://www.votewatch.eu/en/motions-for-resolutions-climate-change-conference-in-durban-motion-for-a-resolution-paragraph-38.html"/>
-    <hyperlink ref="Q8" r:id="rId21" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20111116+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="K9" r:id="rId22" display="http://www.europarl.europa.eu/sides/getDoc.do?type=REPORT&amp;reference=A7-2012-0265&amp;language=EN"/>
-    <hyperlink ref="O9" r:id="rId23" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2012-0306&amp;language=EN&amp;ring=A7-2012-0265"/>
-    <hyperlink ref="P9" r:id="rId24" display="http://www.votewatch.eu/en/energy-efficiency-draft-legislative-resolution-single-vote-ordinary-legislative-procedure-first-read.html"/>
-    <hyperlink ref="Q9" r:id="rId25" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20120911+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="P10" r:id="rId26" display="http://www.votewatch.eu/en/renewable-energy-in-the-european-internal-energy-market-motion-for-resolution-paragraph-1-amendment-.html"/>
-    <hyperlink ref="Q10" r:id="rId27" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130521+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
-    <hyperlink ref="J11" r:id="rId28" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+AMD+B7-2013-0482+011-012+DOC+PDF+V0//EN"/>
-    <hyperlink ref="P11" r:id="rId29" display="http://www.votewatch.eu/en/climate-change-conference-motion-for-resolution-after-paragraph-20-amendment-12-1.html"/>
-    <hyperlink ref="Q11" r:id="rId30" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20131023+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="N2" r:id="rId1" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+AMD+B7-2013-0482+004-010+DOC+PDF+V0//EN"/>
+    <hyperlink ref="T2" r:id="rId2" display="http://www.votewatch.eu/en/climate-change-conference-motion-for-resolution-paragraph-8-amendment-6d.html"/>
+    <hyperlink ref="U2" r:id="rId3" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20131023+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="O4" r:id="rId4" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2009-0089&amp;language=EN&amp;ring=B7-2009-0141"/>
+    <hyperlink ref="O5" r:id="rId5" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2013-0064&amp;language=EN&amp;ring=A7-2012-0191"/>
+    <hyperlink ref="T5" r:id="rId6" display="http://www.votewatch.eu/en/mechanism-for-monitoring-and-reporting-greenhouse-gas-emissions-and-other-information-relevant-to-cl.html"/>
+    <hyperlink ref="U5" r:id="rId7" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130312+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="T4" r:id="rId8" display="http://www.votewatch.eu/en/motion-for-a-resolution-preparation-of-the-copenhagen-summit-on-climate-change-motions-for-a-resolut-19.html"/>
+    <hyperlink ref="U4" r:id="rId9" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20091125+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="T3" r:id="rId10" display="http://www.votewatch.eu/en/competitive-low-carbon-economy-in-2050-motion-for-a-resolution-after-paragraph-1-amendment-1-2.html"/>
+    <hyperlink ref="U3" r:id="rId11" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20120315+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="N6" r:id="rId12" display="http://www.europarl.europa.eu/sides/getDoc.do?type=REPORT&amp;reference=A7-2013-0046&amp;language=EN"/>
+    <hyperlink ref="O6" r:id="rId13" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2013-0310&amp;language=EN&amp;ring=A7-2013-0046"/>
+    <hyperlink ref="T6" r:id="rId14" display="http://www.votewatch.eu/en/timing-of-auctions-of-greenhouse-gas-allowances-draft-legislative-resolution-vote-amended-proposal-o.html"/>
+    <hyperlink ref="U6" r:id="rId15" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130703+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="O7" r:id="rId16" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2011-0430&amp;language=EN&amp;ring=B7-2011-0522"/>
+    <hyperlink ref="T7" r:id="rId17" display="http://www.votewatch.eu/en/motions-for-resolutions-rio-20-earth-summit-motion-for-a-resolution-vote-resolution-text-as-a-whole.html"/>
+    <hyperlink ref="U7" r:id="rId18" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20110929+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="K8" r:id="rId19" display="http://www.europarl.europa.eu/sides/getDoc.do?type=MOTION&amp;reference=B7-2011-0571&amp;language=EN"/>
+    <hyperlink ref="T8" r:id="rId20" display="http://www.votewatch.eu/en/motions-for-resolutions-climate-change-conference-in-durban-motion-for-a-resolution-paragraph-38.html"/>
+    <hyperlink ref="U8" r:id="rId21" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20111116+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="O9" r:id="rId22" display="http://www.europarl.europa.eu/sides/getDoc.do?type=REPORT&amp;reference=A7-2012-0265&amp;language=EN"/>
+    <hyperlink ref="S9" r:id="rId23" display="http://www.europarl.europa.eu/sides/getDoc.do?type=TA&amp;reference=P7-TA-2012-0306&amp;language=EN&amp;ring=A7-2012-0265"/>
+    <hyperlink ref="T9" r:id="rId24" display="http://www.votewatch.eu/en/energy-efficiency-draft-legislative-resolution-single-vote-ordinary-legislative-procedure-first-read.html"/>
+    <hyperlink ref="U9" r:id="rId25" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20120911+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="T10" r:id="rId26" display="http://www.votewatch.eu/en/renewable-energy-in-the-european-internal-energy-market-motion-for-resolution-paragraph-1-amendment-.html"/>
+    <hyperlink ref="U10" r:id="rId27" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20130521+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="N11" r:id="rId28" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+AMD+B7-2013-0482+011-012+DOC+PDF+V0//EN"/>
+    <hyperlink ref="T11" r:id="rId29" display="http://www.votewatch.eu/en/climate-change-conference-motion-for-resolution-after-paragraph-20-amendment-12-1.html"/>
+    <hyperlink ref="U11" r:id="rId30" display="http://www.europarl.europa.eu/sides/getDoc.do?pubRef=-//EP//NONSGML+PV+20131023+RES-RCV+DOC+PDF+V0//EN&amp;language=EN"/>
+    <hyperlink ref="T12" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="48.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="48.21875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>